<commit_message>
Commit Date Thu Jun 23 10:05:40 CEST 2016
</commit_message>
<xml_diff>
--- a/Optimization/GoogleAdWords_LO.xlsx
+++ b/Optimization/GoogleAdWords_LO.xlsx
@@ -1,14 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishna/MOOC/Edge/Optimization/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14080" windowHeight="15020" tabRatio="500"/>
+    <workbookView xWindow="2320" yWindow="460" windowWidth="14080" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$35:$D$37</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$45:$B$47</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$50:$B$52</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$40</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$D$45:$D$47</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$D$50:$D$52</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -163,6 +202,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -490,26 +534,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -523,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -537,7 +581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -551,7 +595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -565,12 +609,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -584,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -598,7 +642,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -612,7 +656,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -626,12 +670,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -645,7 +689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -659,7 +703,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -673,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -687,12 +731,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -700,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -708,7 +752,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -716,7 +760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -724,12 +768,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -737,7 +781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>1</v>
       </c>
@@ -745,7 +789,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>2</v>
       </c>
@@ -753,7 +797,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>3</v>
       </c>
@@ -761,12 +805,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
@@ -780,56 +824,80 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="B35" s="2">
+        <v>40</v>
+      </c>
+      <c r="C35" s="2">
+        <v>40</v>
+      </c>
+      <c r="D35" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="B36" s="2">
+        <v>100</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="B40" s="2">
+        <f>SUMPRODUCT(B35:D37,B17:D19)</f>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="2">
+        <f>SUMPRODUCT(B35:D35,B17:D17)</f>
+        <v>168</v>
+      </c>
       <c r="C45" s="2" t="s">
         <v>21</v>
       </c>
@@ -837,11 +905,14 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2">
+        <f t="shared" ref="B46:B47" si="0">SUMPRODUCT(B36:D36,B18:D18)</f>
+        <v>100</v>
+      </c>
       <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
@@ -849,11 +920,14 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="2">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
       <c r="C47" s="2" t="s">
         <v>21</v>
       </c>
@@ -861,16 +935,19 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="2">
+        <f>SUM(B35:B37)</f>
+        <v>140</v>
+      </c>
       <c r="C50" s="2" t="s">
         <v>21</v>
       </c>
@@ -878,11 +955,14 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="2">
+        <f>SUM(C35:C37)</f>
+        <v>80</v>
+      </c>
       <c r="C51" s="2" t="s">
         <v>21</v>
       </c>
@@ -890,11 +970,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="2">
+        <f>SUM(D35:D37)</f>
+        <v>80</v>
+      </c>
       <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
@@ -904,10 +987,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>